<commit_message>
Added all false cases -> in total 500 cases
</commit_message>
<xml_diff>
--- a/Identiy Resolution/Goldstandard_sales_wiki.xlsx
+++ b/Identiy Resolution/Goldstandard_sales_wiki.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aniek\PycharmProjects\WDI-Project\Identiy Resolution\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA22174-D7D7-4727-AB94-FEA6DBD73CAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22368" yWindow="72" windowWidth="5808" windowHeight="11904"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="500">
   <si>
     <t>sales_12,wiki_16996,TRUE</t>
   </si>
@@ -189,9 +206,6 @@
     <t>sales_9445,wiki_37822,TRUE</t>
   </si>
   <si>
-    <t>sales_10048, wiki_21655,TRUE</t>
-  </si>
-  <si>
     <t>sales_10067,wiki_37221,TRUE</t>
   </si>
   <si>
@@ -406,13 +420,1126 @@
   </si>
   <si>
     <t>sales_84,wiki_22410,TRUE</t>
+  </si>
+  <si>
+    <t>sales_17,wiki_16618,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11,wiki_16606,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12,wiki_16602,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13,wiki_16607,FALSE</t>
+  </si>
+  <si>
+    <t>sales_18,wiki_16620,FALSE</t>
+  </si>
+  <si>
+    <t>sales_21,wiki_16621,FALSE</t>
+  </si>
+  <si>
+    <t>sales_24,wiki_16623,FALSE</t>
+  </si>
+  <si>
+    <t>sales_25,wiki_19471,FALSE</t>
+  </si>
+  <si>
+    <t>sales_26,wiki_19472,FALSE</t>
+  </si>
+  <si>
+    <t>sales_27,wiki_19473,FALSE</t>
+  </si>
+  <si>
+    <t>sales_31,wiki_19474,FALSE</t>
+  </si>
+  <si>
+    <t>sales_33,wiki_19475,FALSE</t>
+  </si>
+  <si>
+    <t>sales_45,wiki_19478,FALSE</t>
+  </si>
+  <si>
+    <t>sales_46,wiki_19480,FALSE</t>
+  </si>
+  <si>
+    <t>sales_50,wiki_19485,FALSE</t>
+  </si>
+  <si>
+    <t>sales_59,wiki_19486,FALSE</t>
+  </si>
+  <si>
+    <t>sales_82,wiki_19487,FALSE</t>
+  </si>
+  <si>
+    <t>sales_85,wiki_19488,FALSE</t>
+  </si>
+  <si>
+    <t>sales_86,wiki_19490,FALSE</t>
+  </si>
+  <si>
+    <t>sales_87,wiki_19492,FALSE</t>
+  </si>
+  <si>
+    <t>sales_121,wiki_17210,FALSE</t>
+  </si>
+  <si>
+    <t>sales_122,wiki_17211,FALSE</t>
+  </si>
+  <si>
+    <t>sales_123,wiki_17215,FALSE</t>
+  </si>
+  <si>
+    <t>sales_125,wiki_17217,FALSE</t>
+  </si>
+  <si>
+    <t>sales_126,wiki_17218,FALSE</t>
+  </si>
+  <si>
+    <t>sales_124,wiki_17216,FALSE</t>
+  </si>
+  <si>
+    <t>sales_127,wiki_17221,FALSE</t>
+  </si>
+  <si>
+    <t>sales_120,wiki_17200,FALSE</t>
+  </si>
+  <si>
+    <t>sales_128,wiki_17222,FALSE</t>
+  </si>
+  <si>
+    <t>sales_129,wiki_17224,FALSE</t>
+  </si>
+  <si>
+    <t>sales_130,wiki_17223,FALSE</t>
+  </si>
+  <si>
+    <t>sales_230,wiki_17346,FALSE</t>
+  </si>
+  <si>
+    <t>sales_231,wiki_17347,FALSE</t>
+  </si>
+  <si>
+    <t>sales_232,wiki_17348,FALSE</t>
+  </si>
+  <si>
+    <t>sales_233,wiki_17704,FALSE</t>
+  </si>
+  <si>
+    <t>sales_234,wiki_17708,FALSE</t>
+  </si>
+  <si>
+    <t>sales_235,wiki_17709,FALSE</t>
+  </si>
+  <si>
+    <t>sales_236,wiki_17710,FALSE</t>
+  </si>
+  <si>
+    <t>sales_237,wiki_17713,FALSE</t>
+  </si>
+  <si>
+    <t>sales_238,wiki_17701,FALSE</t>
+  </si>
+  <si>
+    <t>sales_239,wiki_17703,FALSE</t>
+  </si>
+  <si>
+    <t>sales_240,wiki_17715,FALSE</t>
+  </si>
+  <si>
+    <t>sales_350,wiki_18857,FALSE</t>
+  </si>
+  <si>
+    <t>sales_351,wiki_18844,FALSE</t>
+  </si>
+  <si>
+    <t>sales_352,wiki_18845,FALSE</t>
+  </si>
+  <si>
+    <t>sales_353,wiki_18846,FALSE</t>
+  </si>
+  <si>
+    <t>sales_354,wiki_18847,FALSE</t>
+  </si>
+  <si>
+    <t>sales_355,wiki_18848,FALSE</t>
+  </si>
+  <si>
+    <t>sales_356,wiki_18849,FALSE</t>
+  </si>
+  <si>
+    <t>sales_357,wiki_18850,FALSE</t>
+  </si>
+  <si>
+    <t>sales_358,wiki_18851,FALSE</t>
+  </si>
+  <si>
+    <t>sales_359,wiki_18852,FALSE</t>
+  </si>
+  <si>
+    <t>sales_360,wiki_18853,FALSE</t>
+  </si>
+  <si>
+    <t>sales_470,wiki_19196,FALSE</t>
+  </si>
+  <si>
+    <t>sales_471,wiki_19197,FALSE</t>
+  </si>
+  <si>
+    <t>sales_472,wiki_19198,FALSE</t>
+  </si>
+  <si>
+    <t>sales_473,wiki_19199,FALSE</t>
+  </si>
+  <si>
+    <t>sales_474,wiki_19200,FALSE</t>
+  </si>
+  <si>
+    <t>sales_475,wiki_19201,FALSE</t>
+  </si>
+  <si>
+    <t>sales_476,wiki_19202,FALSE</t>
+  </si>
+  <si>
+    <t>sales_477,wiki_19203,FALSE</t>
+  </si>
+  <si>
+    <t>sales_478,wiki_19204,FALSE</t>
+  </si>
+  <si>
+    <t>sales_479,wiki_19205,FALSE</t>
+  </si>
+  <si>
+    <t>sales_480,wiki_19215,FALSE</t>
+  </si>
+  <si>
+    <t>sales_590,wiki_27469,FALSE</t>
+  </si>
+  <si>
+    <t>sales_592,wiki_27471,FALSE</t>
+  </si>
+  <si>
+    <t>sales_593,wiki_27472,FALSE</t>
+  </si>
+  <si>
+    <t>sales_591,wiki_27470,FALSE</t>
+  </si>
+  <si>
+    <t>sales_594,wiki_27474,FALSE</t>
+  </si>
+  <si>
+    <t>sales_595,wiki_27478,FALSE</t>
+  </si>
+  <si>
+    <t>sales_596,wiki_27480,FALSE</t>
+  </si>
+  <si>
+    <t>sales_597,wiki_27481,FALSE</t>
+  </si>
+  <si>
+    <t>sales_598,wiki_27482,FALSE</t>
+  </si>
+  <si>
+    <t>sales_599,wiki_27483,FALSE</t>
+  </si>
+  <si>
+    <t>sales_600,wiki_27486,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1700,wiki_29542,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1701,wiki_29543,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1702,wiki_29544,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1703,wiki_29545,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1704,wiki_29546,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1705,wiki_29547,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1706,wiki_29548,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1707,wiki_29549,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1708,wiki_29550,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1709,wiki_29551,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1710,wiki_29552,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1850,wiki_29553,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1851,wiki_29554,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1852,wiki_29555,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1853,wiki_29556,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1854,wiki_29557,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1855,wiki_29558,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1856,wiki_29559,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1857,wiki_29560,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1858,wiki_29561,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1859,wiki_29562,FALSE</t>
+  </si>
+  <si>
+    <t>sales_1860,wiki_29563,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2400,wiki_49823,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2401,wiki_49824,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2402,wiki_49825,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2403,wiki_49826,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2404,wiki_49827,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2405,wiki_49828,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2406,wiki_49829,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2407,wiki_49830,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2408,wiki_49831,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2409,wiki_49832,FALSE</t>
+  </si>
+  <si>
+    <t>sales_2410,wiki_49833,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4710,wiki_49834,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4711,wiki_49835,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4712,wiki_49836,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4713,wiki_50318,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4714,wiki_50319,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4715,wiki_50320,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4716,wiki_50321,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4717,wiki_50322,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4718,wiki_50323,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4719,wiki_50324,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4720,wiki_50325,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6820,wiki_51918,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6821,wiki_51919,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6822,wiki_51920,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6823,wiki_51921,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6824,wiki_51922,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6825,wiki_51923,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6826,wiki_51924,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6827,wiki_51925,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6828,wiki_51926,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6829,wiki_51927,FALSE</t>
+  </si>
+  <si>
+    <t>sales_6830,wiki_51928,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7500,wiki_16831,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7501,wiki_16832,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7502,wiki_16833,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7503,wiki_16834,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7504,wiki_16835,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7505,wiki_16836,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7506,wiki_16837,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7507,wiki_16838,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7508,wiki_16839,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7509,wiki_16840,FALSE</t>
+  </si>
+  <si>
+    <t>sales_7510,wiki_16841,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8330,wiki_19030,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8331,wiki_19031,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8332,wiki_19032,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8333,wiki_19033,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8334,wiki_19034,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8335,wiki_19035,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8336,wiki_19036,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8337,wiki_19037,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8338,wiki_19038,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8339,wiki_19039,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8340,wiki_19040,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8341,wiki_19041,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8342,wiki_19042,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8343,wiki_19043,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8344,wiki_19044,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8345,wiki_19045,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8346,wiki_19046,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8347,wiki_19047,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8348,wiki_19048,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8349,wiki_19049,FALSE</t>
+  </si>
+  <si>
+    <t>sales_8350,wiki_19050,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11300,wiki_26289,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11301,wiki_26290,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11302,wiki_26291,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11303,wiki_26292,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11304,wiki_26293,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11305,wiki_26294,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11306,wiki_26295,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11307,wiki_26296,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11308,wiki_26297,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11309,wiki_26298,FALSE</t>
+  </si>
+  <si>
+    <t>sales_11310,wiki_26299,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12550,wiki_27038,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12551,wiki_27039,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12552,wiki_27040,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12553,wiki_27041,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12554,wiki_27042,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12555,wiki_27043,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12556,wiki_27044,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12557,wiki_27045,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12558,wiki_27046,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12559,wiki_27047,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12560,wiki_27048,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12561,wiki_27049,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12562,wiki_27050,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12563,wiki_27051,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12564,wiki_27052,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12565,wiki_27053,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12566,wiki_27054,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12567,wiki_27055,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12568,wiki_27056,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12569,wiki_27057,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12570,wiki_27058,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12801,wiki_23362,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12802,wiki_23363,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12803,wiki_23364,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12804,wiki_23365,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12805,wiki_23366,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12806,wiki_23367,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12807,wiki_23368,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12808,wiki_23369,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12809,wiki_23370,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12810,wiki_23371,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12811,wiki_23372,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12812,wiki_23373,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12813,wiki_23374,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12814,wiki_23375,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12815,wiki_23376,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12816,wiki_23377,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12817,wiki_23378,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12818,wiki_23379,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12819,wiki_23380,FALSE</t>
+  </si>
+  <si>
+    <t>sales_12820,wiki_23381,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13400,wiki_42997,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13401,wiki_42998,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13402,wiki_42999,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13403,wiki_43000,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13404,wiki_43001,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13405,wiki_43002,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13406,wiki_43003,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13407,wiki_43004,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13408,wiki_43005,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13409,wiki_43006,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13410,wiki_43007,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13411,wiki_43008,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13412,wiki_43009,FALSE</t>
+  </si>
+  <si>
+    <t>sales_13413,wiki_43010,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14403,wiki_39632,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14400,wiki_39633,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14401,wiki_39634,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14402,wiki_39635,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14404,wiki_39636,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14405,wiki_39637,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14406,wiki_39638,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14407,wiki_39639,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14408,wiki_39640,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14409,wiki_39641,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14410,wiki_39642,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14411,wiki_39643,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14412,wiki_39644,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14413,wiki_39645,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14414,wiki_39646,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14415,wiki_39647,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14416,wiki_39648,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14417,wiki_39649,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14418,wiki_39650,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14419,wiki_39651,FALSE</t>
+  </si>
+  <si>
+    <t>sales_14420,wiki_39652,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15500,wiki_39723,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15501,wiki_39724,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15502,wiki_39725,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15503,wiki_39726,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15504,wiki_39727,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15505,wiki_39728,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15506,wiki_39729,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15507,wiki_39730,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15508,wiki_39731,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15509,wiki_39732,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15510,wiki_39733,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15511,wiki_39733,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15512,wiki_39734,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15513,wiki_39735,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15514,wiki_39736,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15515,wiki_39737,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15516,wiki_39738,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15517,wiki_39739,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15518,wiki_39740,FALSE</t>
+  </si>
+  <si>
+    <t>sales_15519,wiki_39741,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3300,wiki_41626,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3301,wiki_41627,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3302,wiki_41628,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3303,wiki_41629,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3304,wiki_41630,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3305,wiki_41631,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3306,wiki_41632,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3307,wiki_41633,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3308,wiki_41634,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3309,wiki_41635,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3310,wiki_41636,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3311,wiki_41637,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3312,wiki_41638,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3313,wiki_41639,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3314,wiki_41640,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3315,wiki_41641,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3316,wiki_41642,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3317,wiki_41643,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3318,wiki_41644,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3319,wiki_41645,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3320,wiki_41646,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3830,wiki_26610,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3831,wiki_26611,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3832,wiki_26612,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3833,wiki_26613,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3834,wiki_26614,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3835,wiki_26615,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3836,wiki_26616,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3837,wiki_26617,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3838,wiki_26618,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3839,wiki_26619,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3840,wiki_26620,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3841,wiki_26621,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3842,wiki_26622,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3843,wiki_26623,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3844,wiki_26624,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3845,wiki_26625,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3846,wiki_26626,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3847,wiki_26627,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3848,wiki_26628,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3849,wiki_26629,FALSE</t>
+  </si>
+  <si>
+    <t>sales_3850,wiki_26630,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4260,wiki_18772,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4261,wiki_18773,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4262,wiki_18774,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4263,wiki_18775,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4264,wiki_18776,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4265,wiki_18777,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4266,wiki_18778,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4267,wiki_18779,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4268,wiki_18780,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4269,wiki_18781,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4270,wiki_18782,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4271,wiki_18783,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4272,wiki_18784,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4273,wiki_18785,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4274,wiki_18786,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4275,wiki_18787,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4276,wiki_18788,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4277,wiki_18789,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4278,wiki_18790,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4279,wiki_18791,FALSE</t>
+  </si>
+  <si>
+    <t>sales_4280,wiki_18792,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5100,wiki_19082,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5101,wiki_19083,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5102,wiki_19084,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5103,wiki_19085,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5104,wiki_19086,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5105,wiki_19087,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5106,wiki_19088,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5107,wiki_19089,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5108,wiki_19090,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5109,wiki_19091,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5110,wiki_19092,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5111,wiki_19093,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5112,wiki_19094,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5113,wiki_19095,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5114,wiki_19096,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5115,wiki_19097,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5116,wiki_19098,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5117,wiki_19099,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5118,wiki_19100,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5119,wiki_19101,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5120,wiki_19102,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5801,wiki_39240,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5800,wiki_39241,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5802,wiki_39242,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5803,wiki_39243,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5804,wiki_39244,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5805,wiki_39245,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5806,wiki_39246,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5807,wiki_39247,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5808,wiki_39248,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5809,wiki_39249,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5810,wiki_39250,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5811,wiki_39251,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5812,wiki_39252,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5813,wiki_39253,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5814,wiki_39254,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5815,wiki_39255,FALSE</t>
+  </si>
+  <si>
+    <t>sales_5816,wiki_39256,FALSE</t>
+  </si>
+  <si>
+    <t>sales_10048,wiki_21655,TRUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,13 +1547,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -441,8 +1580,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -453,14 +1593,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -498,9 +1641,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -533,9 +1676,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -568,9 +1728,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -743,11 +1920,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A130"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1039,376 +2216,2227 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>499</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>129</v>
       </c>
     </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A340" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A351" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A362" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A373" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A374" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A375" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A376" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A377" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A378" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A379" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A380" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A384" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A388" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A389" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A390" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A391" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A392" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A394" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A395" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A396" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A398" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A399" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A400" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A401" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A402" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A403" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A405" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A406" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A407" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A408" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A409" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A410" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A411" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A416" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A417" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A422" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A423" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A424" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A425" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A426" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A437" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A438" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A439" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A440" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A441" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A442" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A443" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A444" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A446" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A449" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A450" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A451" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A454" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A457" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A458" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A459" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A460" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A461" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A462" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A463" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A464" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A465" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A466" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A467" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A468" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A469" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A470" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A471" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A472" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A473" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A474" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A475" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A476" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A477" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A478" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A479" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A480" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A481" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A482" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A483" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A484" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A485" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A486" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A487" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A488" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A489" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A490" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A491" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A492" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A493" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A494" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A495" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A496" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A497" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A498" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A499" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A500" t="s">
+        <v>397</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1420,7 +4448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>